<commit_message>
[pr4-2874] XML schema for dictionaries: Data is imported correctly. Open issues  the new schema must be applied to the xlsx file and data exported. Issue #: 2874
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>Title</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>CFTProductivityRateMax</t>
-  </si>
-  <si>
-    <t>CFTProductivityNormMin</t>
-  </si>
-  <si>
-    <t>CFTProductivityNormMax</t>
   </si>
   <si>
     <t>Współczynnik</t>
@@ -671,9 +665,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:E2" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:C2" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
+  <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
       <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
@@ -682,12 +676,6 @@
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:CFTProductivityRateMax" name="CFTProductivityRateMax">
       <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMax" xmlDataType="double"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="ns1:CFTProductivityNormMin" name="CFTProductivityNormMin">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityNormMin" xmlDataType="double"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="ns1:CFTProductivityNormMax" name="CFTProductivityNormMax">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityNormMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1077,15 +1065,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1">
         <v>84</v>
@@ -1096,7 +1084,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1">
         <v>99</v>
@@ -1107,7 +1095,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1">
         <v>65</v>
@@ -1118,7 +1106,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1">
         <v>69</v>
@@ -1129,7 +1117,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1">
         <v>99</v>
@@ -1140,7 +1128,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1">
         <v>99</v>
@@ -1151,7 +1139,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -1162,7 +1150,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1198,223 +1186,223 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1457,7 +1445,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1503,7 +1491,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1557,10 +1545,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1623,7 +1611,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3">
         <v>572</v>
@@ -1637,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4">
         <v>839</v>
@@ -1651,7 +1639,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5">
         <v>729</v>
@@ -1665,7 +1653,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>871</v>
@@ -1679,7 +1667,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7">
         <v>551</v>
@@ -1693,7 +1681,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>394</v>
@@ -1707,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>756</v>
@@ -1726,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1737,11 +1725,9 @@
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.375" customWidth="1"/>
     <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1751,28 +1737,16 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B2" s="3">
         <v>0.98499999999999999</v>
       </c>
       <c r="C2" s="3">
         <v>0.995</v>
-      </c>
-      <c r="D2" s="3">
-        <v>9.8499999999999998E-4</v>
-      </c>
-      <c r="E2" s="3">
-        <v>9.9500000000000001E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1806,27 +1780,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>40877</v>
@@ -1870,69 +1844,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1947,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1964,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1975,16 +1949,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2762] IPR: Create SPMetal configuration - synchronized with the current information model of the website. Issue #: 2762
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>Title</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>ProductCodeNumber</t>
-  </si>
-  <si>
-    <t>ProductName</t>
   </si>
   <si>
     <t>Compensation Good</t>
@@ -710,17 +707,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A1:D5" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:D5"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A1:C5" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:C5"/>
+  <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
       <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ProductCodeNumber" name="ProductCodeNumber">
       <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductCodeNumber" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:ProductName" name="ProductName">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:CompensationGood" name="Compensation Good">
       <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:CompensationGood" xmlDataType="string"/>
@@ -1065,15 +1059,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1">
         <v>84</v>
@@ -1084,7 +1078,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1">
         <v>99</v>
@@ -1095,7 +1089,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1">
         <v>65</v>
@@ -1106,7 +1100,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1">
         <v>69</v>
@@ -1117,7 +1111,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1">
         <v>99</v>
@@ -1128,7 +1122,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1">
         <v>99</v>
@@ -1139,7 +1133,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -1150,7 +1144,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1186,223 +1180,223 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1439,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1491,7 +1485,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1545,10 +1539,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1611,7 +1605,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>572</v>
@@ -1625,7 +1619,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>839</v>
@@ -1639,7 +1633,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>729</v>
@@ -1653,7 +1647,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>871</v>
@@ -1667,7 +1661,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7">
         <v>551</v>
@@ -1681,7 +1675,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>394</v>
@@ -1695,7 +1689,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <v>756</v>
@@ -1716,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1797,7 +1791,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -1825,21 +1819,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="29.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,41 +1842,32 @@
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
@@ -1891,22 +1875,16 @@
       <c r="C4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1949,16 +1927,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2896] Harmonize Configuration schema with the current information model. schema, excel, export done. Publication error for Format lib. Issue #: 2896
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -390,9 +390,9 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="xmlns:ns1='http://cas.eu/schemas/jti/ipr/Batch.xsd'">
-  <Schema ID="Schema1" Namespace="http://cas.eu/schemas/jti/ipr/Batch.xsd">
+  <Schema ID="Schema2" Namespace="http://cas.eu/schemas/jti/ipr/Batch.xsd">
     <xsd:schema xmlns="http://cas.eu/schemas/jti/ipr/Batch.xsd" xmlns:mstns="http://cas.eu/schemas/jti/ipr/Batch.xsd" xmlns:xsd="http://www.w3.org/2001/XMLSchema" id="Configuration" targetNamespace="http://cas.eu/schemas/jti/ipr/Batch.xsd" elementFormDefault="qualified">
-      <xsd:element name="Configuratio">
+      <xsd:element name="Configuration">
         <xsd:complexType>
           <xsd:sequence>
             <xsd:element nillable="true" minOccurs="0" name="Format">
@@ -478,8 +478,8 @@
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Title"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityRateMin"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityRateMax"/>
-                        <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMin"/>
-                        <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMax"/>
+                        <!--<xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMin"/>
+                    <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMax"/>-->
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -512,7 +512,6 @@
                       <xsd:sequence minOccurs="0">
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Title"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ProductCodeNumber"/>
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ProductName"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CompensationGood"/>
                       </xsd:sequence>
                     </xsd:complexType>
@@ -555,7 +554,7 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="17" Name="Configuratio_mapa" RootElement="Configuratio" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="18" Name="Configuration_mapa" RootElement="Configuration" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
@@ -564,13 +563,13 @@
   <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Format/ns1:FormatItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:CigaretteLenght" name="CigaretteLenght">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Format/ns1:FormatItem/ns1:CigaretteLenght" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:CigaretteLenght" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:FilterLenght" name="FilterLenght">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Format/ns1:FormatItem/ns1:FilterLenght" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:FilterLenght" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -582,10 +581,10 @@
   <autoFilter ref="A1:B28"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:EUPrimeMarket" name="EU Prime Market">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:EUPrimeMarket" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:EUPrimeMarket" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -597,10 +596,10 @@
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Waste/ns1:WasteItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:WasteRatio" name="WasteRatio">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Waste/ns1:WasteItem/ns1:WasteRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:WasteRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -612,10 +611,10 @@
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Dust/ns1:DustItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:DustRatio" name="DustRatio">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Dust/ns1:DustItem/ns1:DustRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:DustRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -627,13 +626,13 @@
   <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:SHMenthol/ns1:SHMentholItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:SHMenthol/ns1:SHMentholItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:SHMentholRatio" name="SHMentholRatio">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:SHMenthol/ns1:SHMentholItem/ns1:SHMentholRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:SHMentholRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -645,16 +644,16 @@
   <autoFilter ref="A1:D9"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Usage/ns1:UsageItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:Format_lookup" name="Format lookup">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Usage/ns1:UsageItem/ns1:Format_lookup" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Format_lookup" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:UsageMin" name="UsageMin">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Usage/ns1:UsageItem/ns1:UsageMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:UsageMax" name="UsageMax">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Usage/ns1:UsageItem/ns1:UsageMax" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -666,13 +665,13 @@
   <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:CFTProductivityRateMin" name="CFTProductivityRateMin">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:CFTProductivityRateMax" name="CFTProductivityRateMax">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMax" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -684,22 +683,22 @@
   <autoFilter ref="A1:F2"/>
   <tableColumns count="6">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ConsentNo" name="ConsentNo">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:ValidFromDate" name="Valid from date" dataDxfId="1">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:ValidFromDate" xmlDataType="date"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidFromDate" xmlDataType="date"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:ValidToDate" name="Valid to date" dataDxfId="0">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:ValidToDate" xmlDataType="date"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidToDate" xmlDataType="date"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="ns1:ProductivityRateMin" name="Productivity rate - min">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="ns1:ProductivityRateMax" name="Productivity rate - max">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMax" xmlDataType="double"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -711,13 +710,13 @@
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ProductCodeNumber" name="ProductCodeNumber">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductCodeNumber" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductCodeNumber" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:CompensationGood" name="Compensation Good">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:PCNCode/ns1:PCNCodeItem/ns1:CompensationGood" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:CompensationGood" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -729,16 +728,16 @@
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Warehouse/ns1:WarehouseItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:External" name="External">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Warehouse/ns1:WarehouseItem/ns1:External" xmlDataType="boolean"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:External" xmlDataType="boolean"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Warehouse/ns1:WarehouseItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:ItemType" name="Item Type">
-      <xmlColumnPr mapId="17" xpath="/ns1:Configuratio/ns1:Warehouse/ns1:WarehouseItem/ns1:ItemType" xmlDataType="string"/>
+      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ItemType" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1165,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
@@ -1458,7 +1457,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1561,7 +1560,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1711,7 +1710,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1756,7 +1755,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1821,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[pr4-2896] Harmonize Configuration schema with the current information model. Done and works. Issue #: 2896
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>Title</t>
   </si>
@@ -316,15 +316,9 @@
     <t>kartony z tektury falistej</t>
   </si>
   <si>
-    <t>kartony</t>
-  </si>
-  <si>
     <t>krajanka tytoniowa krótkowółknista</t>
   </si>
   <si>
-    <t>krajanka</t>
-  </si>
-  <si>
     <t>War</t>
   </si>
   <si>
@@ -332,6 +326,15 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>Papierosy</t>
+  </si>
+  <si>
+    <t>PyłTytoiowy</t>
+  </si>
+  <si>
+    <t>Kartony</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
@@ -1820,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1850,7 +1853,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1861,7 +1864,7 @@
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1872,18 +1875,18 @@
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1926,16 +1929,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2907] Add Consent.ConsentPeriod to the configuration Issue #: 2907
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
   <si>
     <t>Title</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Cutfiller</t>
-  </si>
-  <si>
-    <t>18</t>
   </si>
   <si>
     <t>2402209000</t>
@@ -682,12 +679,9 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:F2" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:F2"/>
-  <tableColumns count="6">
-    <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:Title" xmlDataType="string"/>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:E2" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
+  <tableColumns count="5">
     <tableColumn id="2" uniqueName="ns1:ConsentNo" name="ConsentNo">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
     </tableColumn>
@@ -1755,59 +1749,52 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
-    <col min="6" max="6" width="29.25" customWidth="1"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="29.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B2" s="2">
+        <v>40877</v>
+      </c>
       <c r="C2" s="2">
-        <v>40877</v>
-      </c>
-      <c r="D2" s="2">
         <v>41145</v>
       </c>
+      <c r="D2" s="3">
+        <v>0.97</v>
+      </c>
       <c r="E2" s="3">
-        <v>0.97</v>
-      </c>
-      <c r="F2" s="3">
         <v>1.1200000000000001</v>
       </c>
     </row>
@@ -1823,7 +1810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1850,37 +1837,37 @@
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
@@ -1929,16 +1916,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2897] Usage.Title column should be removed - schema excel done Issue #: 2897
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>Title</t>
   </si>
@@ -64,9 +64,6 @@
     <t>UsageMax</t>
   </si>
   <si>
-    <t>Usage</t>
-  </si>
-  <si>
     <t>CFTProductivityRateMin</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Kartony</t>
+  </si>
+  <si>
+    <t>ConsentPeriod</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,10 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
     </dxf>
@@ -640,12 +643,9 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:D9" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
-  <tableColumns count="4">
-    <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Title" xmlDataType="string"/>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:C9" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:C9"/>
+  <tableColumns count="3">
     <tableColumn id="2" uniqueName="ns1:Format_lookup" name="Format lookup">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Format_lookup" xmlDataType="string"/>
     </tableColumn>
@@ -679,16 +679,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:E2" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:F2" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:F2">
+    <filterColumn colId="5"/>
+  </autoFilter>
+  <tableColumns count="6">
     <tableColumn id="2" uniqueName="ns1:ConsentNo" name="ConsentNo">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:ValidFromDate" name="Valid from date" dataDxfId="1">
+    <tableColumn id="3" uniqueName="ns1:ValidFromDate" name="Valid from date" dataDxfId="2">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidFromDate" xmlDataType="date"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="ns1:ValidToDate" name="Valid to date" dataDxfId="0">
+    <tableColumn id="4" uniqueName="ns1:ValidToDate" name="Valid to date" dataDxfId="1">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidToDate" xmlDataType="date"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="ns1:ProductivityRateMin" name="Productivity rate - min">
@@ -697,6 +699,7 @@
     <tableColumn id="6" uniqueName="ns1:ProductivityRateMax" name="Productivity rate - max">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMax" xmlDataType="double"/>
     </tableColumn>
+    <tableColumn id="7" uniqueName="7" name="ConsentPeriod" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1055,15 +1058,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1">
         <v>84</v>
@@ -1074,7 +1077,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1">
         <v>99</v>
@@ -1085,7 +1088,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1">
         <v>65</v>
@@ -1096,7 +1099,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1">
         <v>69</v>
@@ -1107,7 +1110,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1">
         <v>99</v>
@@ -1118,7 +1121,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1">
         <v>99</v>
@@ -1129,7 +1132,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -1140,7 +1143,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1176,223 +1179,223 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1435,7 +1438,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1481,7 +1484,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1535,10 +1538,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1554,143 +1557,115 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="10.75" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="3">
+        <v>666</v>
+      </c>
       <c r="C2" s="3">
-        <v>666</v>
-      </c>
-      <c r="D2" s="3">
         <v>759</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <v>572</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C3">
-        <v>572</v>
-      </c>
-      <c r="D3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4">
+        <v>839</v>
+      </c>
+      <c r="C4">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C4">
-        <v>839</v>
-      </c>
-      <c r="D4">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5">
+        <v>729</v>
+      </c>
+      <c r="C5">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C5">
-        <v>729</v>
-      </c>
-      <c r="D5">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6">
+        <v>871</v>
+      </c>
+      <c r="C6">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C6">
-        <v>871</v>
-      </c>
-      <c r="D6">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7">
+        <v>551</v>
+      </c>
+      <c r="C7">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C7">
-        <v>551</v>
-      </c>
-      <c r="D7">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8">
+        <v>394</v>
+      </c>
+      <c r="C8">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C8">
-        <v>394</v>
-      </c>
-      <c r="D8">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
+      <c r="B9">
+        <v>756</v>
       </c>
       <c r="C9">
-        <v>756</v>
-      </c>
-      <c r="D9">
         <v>901</v>
       </c>
     </row>
@@ -1722,15 +1697,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
         <v>0.98499999999999999</v>
@@ -1749,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1761,29 +1736,33 @@
     <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
     <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="29.25" customWidth="1"/>
+    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B2" s="2">
         <v>40877</v>
@@ -1796,6 +1775,9 @@
       </c>
       <c r="E2" s="3">
         <v>1.1200000000000001</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1826,54 +1808,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1916,16 +1898,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2911] CutfillerCoefficient.Title remove from configuration - schema and  excel done. Issue #: 2911
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
   <si>
     <t>Title</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>CFTProductivityRateMax</t>
-  </si>
-  <si>
-    <t>Współczynnik</t>
   </si>
   <si>
     <t>ConsentNo</t>
@@ -661,12 +658,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:C2" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
-  <tableColumns count="3">
-    <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:Title" xmlDataType="string"/>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:B2" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:B2"/>
+  <tableColumns count="2">
     <tableColumn id="2" uniqueName="ns1:CFTProductivityRateMin" name="CFTProductivityRateMin">
       <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMin" xmlDataType="double"/>
     </tableColumn>
@@ -1058,15 +1052,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1">
         <v>84</v>
@@ -1077,7 +1071,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1">
         <v>99</v>
@@ -1088,7 +1082,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1">
         <v>65</v>
@@ -1099,7 +1093,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1">
         <v>69</v>
@@ -1110,7 +1104,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1">
         <v>99</v>
@@ -1121,7 +1115,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1">
         <v>99</v>
@@ -1132,7 +1126,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -1143,7 +1137,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1179,223 +1173,223 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1438,7 +1432,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1484,7 +1478,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1538,10 +1532,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1559,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1594,7 +1588,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>572</v>
@@ -1605,7 +1599,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>839</v>
@@ -1616,7 +1610,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>729</v>
@@ -1627,7 +1621,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>871</v>
@@ -1638,7 +1632,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7">
         <v>551</v>
@@ -1649,7 +1643,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>394</v>
@@ -1660,7 +1654,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9">
         <v>756</v>
@@ -1679,38 +1673,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.375" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
+    <col min="1" max="1" width="22.375" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3">
+        <v>0.98499999999999999</v>
       </c>
       <c r="B2" s="3">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="C2" s="3">
         <v>0.995</v>
       </c>
     </row>
@@ -1742,27 +1729,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>40877</v>
@@ -1808,54 +1795,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1887,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -1898,16 +1885,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[pr4-2913] Remap xlsx and export data - done, next step AK QA Issue #: 2913
</commit_message>
<xml_diff>
--- a/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
+++ b/VS/trunk/PR42-SmartFactory/XML/Dictionaries/JTIConfigurationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="15840" windowHeight="8985" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
   <si>
     <t>Title</t>
   </si>
@@ -265,12 +265,6 @@
     <t>IT</t>
   </si>
   <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>King Size 84/27</t>
   </si>
   <si>
@@ -326,6 +320,36 @@
   </si>
   <si>
     <t>Kartony</t>
+  </si>
+  <si>
+    <t>84.00 mm</t>
+  </si>
+  <si>
+    <t>21.00 mm</t>
+  </si>
+  <si>
+    <t>27.00 mm</t>
+  </si>
+  <si>
+    <t>99.00 mm</t>
+  </si>
+  <si>
+    <t>25.00 mm</t>
+  </si>
+  <si>
+    <t>65.00 mm</t>
+  </si>
+  <si>
+    <t>100.00 mm</t>
+  </si>
+  <si>
+    <t>69.00 mm</t>
+  </si>
+  <si>
+    <t>30.00 mm</t>
+  </si>
+  <si>
+    <t>0.00 mm</t>
   </si>
   <si>
     <t>ConsentPeriod</t>
@@ -385,12 +409,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="xmlns:ns1='http://cas.eu/schemas/jti/ipr/Batch.xsd'">
-  <Schema ID="Schema2" Namespace="http://cas.eu/schemas/jti/ipr/Batch.xsd">
+  <Schema ID="Schema3" Namespace="http://cas.eu/schemas/jti/ipr/Batch.xsd">
     <xsd:schema xmlns="http://cas.eu/schemas/jti/ipr/Batch.xsd" xmlns:mstns="http://cas.eu/schemas/jti/ipr/Batch.xsd" xmlns:xsd="http://www.w3.org/2001/XMLSchema" id="Configuration" targetNamespace="http://cas.eu/schemas/jti/ipr/Batch.xsd" elementFormDefault="qualified">
       <xsd:element name="Configuration">
         <xsd:complexType>
@@ -459,7 +488,6 @@
                   <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="UsageItem">
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Title"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Format_lookup"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="UsageMin"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="UsageMax"/>
@@ -475,11 +503,8 @@
                   <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="CutfillerCoefficientItem">
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Title"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityRateMin"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityRateMax"/>
-                        <!--<xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMin"/>
-                    <xsd:element minOccurs="1" type="xsd:double" name="CFTProductivityNormMax"/>-->
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -492,12 +517,12 @@
                   <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="ConsentItem">
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
-                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Title"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConsentNo"/>
                         <xsd:element minOccurs="0" type="xsd:date" name="ValidFromDate"/>
                         <xsd:element minOccurs="0" type="xsd:date" name="ValidToDate"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="ProductivityRateMin"/>
                         <xsd:element minOccurs="1" type="xsd:double" name="ProductivityRateMax"/>
+                        <xsd:element minOccurs="1" type="xsd:double" name="ConsentPeriod"/>
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -554,7 +579,7 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="18" Name="Configuration_mapa" RootElement="Configuration" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="19" Name="Configuration_mapa" RootElement="Configuration" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
@@ -563,13 +588,13 @@
   <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:CigaretteLenght" name="CigaretteLenght">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:CigaretteLenght" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:CigaretteLenght" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:FilterLenght" name="FilterLenght">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:FilterLenght" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Format/ns1:FormatItem/ns1:FilterLenght" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -581,10 +606,10 @@
   <autoFilter ref="A1:B28"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:EUPrimeMarket" name="EU Prime Market">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:EUPrimeMarket" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:CustomsUnion/ns1:CustomsUnionItem/ns1:EUPrimeMarket" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -596,10 +621,10 @@
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:WasteRatio" name="WasteRatio">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:WasteRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Waste/ns1:WasteItem/ns1:WasteRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -611,10 +636,10 @@
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:DustRatio" name="DustRatio">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:DustRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Dust/ns1:DustItem/ns1:DustRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -626,13 +651,13 @@
   <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:SHMentholRatio" name="SHMentholRatio">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:SHMentholRatio" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:SHMenthol/ns1:SHMentholItem/ns1:SHMentholRatio" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -640,17 +665,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:C9" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:C10" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
     <tableColumn id="2" uniqueName="ns1:Format_lookup" name="Format lookup">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Format_lookup" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:Format_lookup" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:UsageMin" name="UsageMin">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:UsageMax" name="UsageMax">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMax" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Usage/ns1:UsageItem/ns1:UsageMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -662,10 +687,10 @@
   <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
     <tableColumn id="2" uniqueName="ns1:CFTProductivityRateMin" name="CFTProductivityRateMin">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:CFTProductivityRateMax" name="CFTProductivityRateMax">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMax" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:CutfillerCoefficient/ns1:CutfillerCoefficientItem/ns1:CFTProductivityRateMax" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -679,21 +704,23 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="2" uniqueName="ns1:ConsentNo" name="ConsentNo">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentNo" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:ValidFromDate" name="Valid from date" dataDxfId="2">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidFromDate" xmlDataType="date"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidFromDate" xmlDataType="date"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:ValidToDate" name="Valid to date" dataDxfId="1">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidToDate" xmlDataType="date"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ValidToDate" xmlDataType="date"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="ns1:ProductivityRateMin" name="Productivity rate - min">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMin" xmlDataType="double"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMin" xmlDataType="double"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="ns1:ProductivityRateMax" name="Productivity rate - max">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMax" xmlDataType="double"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="7" name="ConsentPeriod" dataDxfId="0"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ProductivityRateMax" xmlDataType="double"/>
+    </tableColumn>
+    <tableColumn id="1" uniqueName="ns1:ConsentPeriod" name="ConsentPeriod" dataDxfId="0">
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Consent/ns1:ConsentItem/ns1:ConsentPeriod" xmlDataType="double"/>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,13 +731,13 @@
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:ProductCodeNumber" name="ProductCodeNumber">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductCodeNumber" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:ProductCodeNumber" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:CompensationGood" name="Compensation Good">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:CompensationGood" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:PCNCode/ns1:PCNCodeItem/ns1:CompensationGood" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -722,16 +749,16 @@
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="ns1:Title" name="Title">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:Title" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:Title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ns1:External" name="External">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:External" xmlDataType="boolean"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:External" xmlDataType="boolean"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="ns1:ProductType" name="ProductType">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ProductType" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ProductType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="ns1:ItemType" name="Item Type">
-      <xmlColumnPr mapId="18" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ItemType" xmlDataType="string"/>
+      <xmlColumnPr mapId="19" xpath="/ns1:Configuration/ns1:Warehouse/ns1:WarehouseItem/ns1:ItemType" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1026,7 +1053,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1052,98 +1079,98 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="1">
-        <v>84</v>
-      </c>
-      <c r="C3" s="1">
-        <v>27</v>
+        <v>80</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="1">
-        <v>99</v>
-      </c>
-      <c r="C4" s="1">
-        <v>25</v>
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="1">
-        <v>65</v>
-      </c>
-      <c r="C5" s="1">
-        <v>100</v>
+        <v>82</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="1">
-        <v>69</v>
-      </c>
-      <c r="C6" s="1">
-        <v>100</v>
+        <v>83</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="1">
-        <v>99</v>
-      </c>
-      <c r="C7" s="1">
-        <v>27</v>
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="1">
-        <v>99</v>
-      </c>
-      <c r="C8" s="1">
-        <v>30</v>
+        <v>85</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="1">
-        <v>100</v>
-      </c>
-      <c r="C9" s="1">
-        <v>27</v>
+        <v>86</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
@@ -1432,7 +1459,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1478,7 +1505,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1532,10 +1559,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1551,7 +1578,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -1588,7 +1615,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>572</v>
@@ -1599,7 +1626,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>839</v>
@@ -1610,7 +1637,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>729</v>
@@ -1621,7 +1648,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>871</v>
@@ -1632,7 +1659,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>551</v>
@@ -1643,7 +1670,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>394</v>
@@ -1654,13 +1681,24 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>756</v>
       </c>
       <c r="C9">
         <v>901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1675,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1695,10 +1733,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3">
-        <v>0.98499999999999999</v>
+        <v>98.5</v>
       </c>
       <c r="B2" s="3">
-        <v>0.995</v>
+        <v>99.5</v>
       </c>
     </row>
   </sheetData>
@@ -1723,8 +1761,7 @@
     <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
     <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="5" max="6" width="29.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1744,7 +1781,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1758,10 +1795,10 @@
         <v>41145</v>
       </c>
       <c r="D2" s="3">
-        <v>0.97</v>
+        <v>97</v>
       </c>
       <c r="E2" s="3">
-        <v>1.1200000000000001</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -1779,7 +1816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1806,43 +1843,43 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1">
         <v>2401300000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1">
         <v>4819100000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1">
         <v>2403999000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1885,16 +1922,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>